<commit_message>
need to slice the data differently
</commit_message>
<xml_diff>
--- a/rapid/country-data.xlsx
+++ b/rapid/country-data.xlsx
@@ -1668,7 +1668,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C195" sqref="C195"/>
+      <selection pane="bottomLeft" activeCell="E194" sqref="E194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
@@ -6348,17 +6348,17 @@
         <v>405</v>
       </c>
       <c r="C195" s="12">
-        <v>30000000</v>
+        <v>23780000</v>
       </c>
       <c r="D195" s="8">
-        <v>8078.7904743723802</v>
+        <v>25026</v>
       </c>
       <c r="E195" s="9">
         <f t="shared" si="6"/>
-        <v>5.0210009163283909</v>
+        <v>15.553760099440646</v>
       </c>
       <c r="F195" s="6" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G195" s="10" t="s">
         <v>29</v>
@@ -6372,14 +6372,14 @@
         <v>406</v>
       </c>
       <c r="C196" s="12">
-        <v>1500000</v>
+        <v>4817000</v>
       </c>
       <c r="D196" s="8">
-        <v>3525.02016450058</v>
+        <v>3094.73</v>
       </c>
       <c r="E196" s="9">
         <f t="shared" si="6"/>
-        <v>2.1908142725298818</v>
+        <v>1.9233871970167806</v>
       </c>
       <c r="F196" s="6" t="s">
         <v>20</v>
@@ -6390,7 +6390,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>